<commit_message>
modifications to account for provincial data
</commit_message>
<xml_diff>
--- a/Ag Eto model/NWSAS_crop_calendar.xlsx
+++ b/Ag Eto model/NWSAS_crop_calendar.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="First Sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="all crops" sheetId="4" r:id="rId2"/>
+    <sheet name="All crops" sheetId="6" r:id="rId2"/>
     <sheet name="data palms info" sheetId="3" r:id="rId3"/>
     <sheet name="Vegetables" sheetId="2" r:id="rId4"/>
     <sheet name="olives" sheetId="5" r:id="rId5"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="154">
   <si>
     <t>Mode</t>
   </si>
@@ -417,9 +417,6 @@
     <t>30/06</t>
   </si>
   <si>
-    <t>wheat</t>
-  </si>
-  <si>
     <t>01/12</t>
   </si>
   <si>
@@ -683,6 +680,12 @@
   </si>
   <si>
     <t xml:space="preserve">assumption </t>
+  </si>
+  <si>
+    <t>vegetables</t>
+  </si>
+  <si>
+    <t>wheat</t>
   </si>
 </sst>
 </file>
@@ -1667,7 +1670,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1684,7 +1687,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B1" s="66" t="s">
         <v>27</v>
@@ -1740,9 +1743,34 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
+    <row r="3" spans="1:9" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="76" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="74" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="75" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" s="74" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="75" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" s="74" t="s">
+        <v>108</v>
+      </c>
+      <c r="I3" s="75" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1756,24 +1784,17 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:I5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="11.81640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" customWidth="1"/>
-    <col min="9" max="9" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.81640625" style="3"/>
+    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="B1" s="66" t="s">
         <v>27</v>
@@ -1801,7 +1822,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="76" t="s">
         <v>94</v>
       </c>
       <c r="B2" s="74" t="s">
@@ -1831,89 +1852,89 @@
     </row>
     <row r="3" spans="1:9" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="76" t="s">
-        <v>103</v>
+        <v>152</v>
       </c>
       <c r="B3" s="74" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="74" t="s">
+      <c r="E3" s="75" t="s">
         <v>105</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="F3" s="74" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="74" t="s">
+      <c r="G3" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="75" t="s">
+      <c r="H3" s="74" t="s">
         <v>108</v>
-      </c>
-      <c r="H3" s="74" t="s">
-        <v>109</v>
       </c>
       <c r="I3" s="75" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="76" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="74" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="75" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="75" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="74" t="s">
+        <v>139</v>
+      </c>
+      <c r="G4" s="75" t="s">
+        <v>140</v>
+      </c>
+      <c r="H4" s="74" t="s">
+        <v>141</v>
+      </c>
+      <c r="I4" s="75" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="75" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="74" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="74" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="75" t="s">
-        <v>95</v>
-      </c>
-      <c r="D4" s="74" t="s">
-        <v>102</v>
-      </c>
-      <c r="E4" s="75" t="s">
+      <c r="E5" s="75" t="s">
         <v>96</v>
       </c>
-      <c r="F4" s="74" t="s">
+      <c r="F5" s="74" t="s">
         <v>97</v>
       </c>
-      <c r="G4" s="75" t="s">
+      <c r="G5" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="H4" s="74" t="s">
+      <c r="H5" s="74" t="s">
         <v>99</v>
       </c>
-      <c r="I4" s="75" t="s">
+      <c r="I5" s="75" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="76" t="s">
-        <v>134</v>
-      </c>
-      <c r="B5" s="74" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="75" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="74" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="75" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" s="74" t="s">
-        <v>140</v>
-      </c>
-      <c r="G5" s="75" t="s">
-        <v>141</v>
-      </c>
-      <c r="H5" s="74" t="s">
-        <v>142</v>
-      </c>
-      <c r="I5" s="75" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1925,8 +1946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2699,7 +2720,7 @@
   <dimension ref="B2:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:K21"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2714,7 +2735,7 @@
     </row>
     <row r="3" spans="2:9" ht="13" x14ac:dyDescent="0.3">
       <c r="C3" s="83" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -2723,13 +2744,13 @@
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" s="85" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="85" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -2737,13 +2758,13 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C8" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="84" t="s">
         <v>113</v>
       </c>
-      <c r="D8" s="84" t="s">
+      <c r="E8" s="84" t="s">
         <v>114</v>
-      </c>
-      <c r="E8" s="84" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
@@ -2762,35 +2783,35 @@
     </row>
     <row r="12" spans="2:9" ht="13" x14ac:dyDescent="0.3">
       <c r="C12" s="83" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.4">
       <c r="C13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" t="s">
         <v>119</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>120</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>121</v>
-      </c>
-      <c r="F13" t="s">
-        <v>122</v>
       </c>
       <c r="G13" t="s">
         <v>16</v>
       </c>
       <c r="H13" t="s">
+        <v>122</v>
+      </c>
+      <c r="I13" t="s">
         <v>123</v>
-      </c>
-      <c r="I13" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="87" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C14" s="86">
         <v>25</v>
@@ -2808,18 +2829,18 @@
         <v>130</v>
       </c>
       <c r="H14" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" t="s">
         <v>117</v>
-      </c>
-      <c r="I14" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="87" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" s="88" t="s">
         <v>127</v>
-      </c>
-      <c r="C16" s="88" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.25">
@@ -2827,13 +2848,13 @@
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C18" s="87" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="3:11" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="3:11" ht="13" x14ac:dyDescent="0.3">
       <c r="C20" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D20" s="66" t="s">
         <v>27</v>
@@ -2862,28 +2883,28 @@
     </row>
     <row r="21" spans="3:11" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="76" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D21" s="74" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="F21" s="74" t="s">
+      <c r="G21" s="75" t="s">
         <v>105</v>
       </c>
-      <c r="G21" s="75" t="s">
+      <c r="H21" s="74" t="s">
         <v>106</v>
       </c>
-      <c r="H21" s="74" t="s">
+      <c r="I21" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="I21" s="75" t="s">
+      <c r="J21" s="74" t="s">
         <v>108</v>
-      </c>
-      <c r="J21" s="74" t="s">
-        <v>109</v>
       </c>
       <c r="K21" s="75" t="s">
         <v>4</v>
@@ -2891,23 +2912,23 @@
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C24" s="84" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D25" s="87" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C26" s="87" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D26" s="87" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E26" s="89" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2924,8 +2945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2939,26 +2960,26 @@
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C2" s="91" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C4" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="84" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="84" t="s">
+      <c r="E4" s="84" t="s">
         <v>114</v>
       </c>
-      <c r="E4" s="84" t="s">
-        <v>115</v>
-      </c>
       <c r="G4" s="85" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C5" s="84" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D5" s="84" t="s">
         <v>93</v>
@@ -2967,12 +2988,12 @@
         <v>93</v>
       </c>
       <c r="G5" s="88" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="92" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C6" s="86">
         <v>0.45</v>
@@ -2984,10 +3005,10 @@
         <v>0.6</v>
       </c>
       <c r="F6" s="92" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G6" s="93" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
@@ -3001,31 +3022,31 @@
     </row>
     <row r="11" spans="2:12" ht="15" x14ac:dyDescent="0.4">
       <c r="D11" s="86" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="86" t="s">
         <v>119</v>
       </c>
-      <c r="E11" s="86" t="s">
+      <c r="F11" s="86" t="s">
         <v>120</v>
       </c>
-      <c r="F11" s="86" t="s">
+      <c r="G11" s="86" t="s">
         <v>121</v>
-      </c>
-      <c r="G11" s="86" t="s">
-        <v>122</v>
       </c>
       <c r="H11" s="86" t="s">
         <v>16</v>
       </c>
       <c r="I11" s="86" t="s">
+        <v>122</v>
+      </c>
+      <c r="J11" s="86" t="s">
         <v>123</v>
-      </c>
-      <c r="J11" s="86" t="s">
-        <v>124</v>
       </c>
       <c r="L11" s="86"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C12" s="86" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D12" s="86">
         <v>30</v>
@@ -3043,10 +3064,10 @@
         <v>270</v>
       </c>
       <c r="I12" s="86" t="s">
+        <v>137</v>
+      </c>
+      <c r="J12" s="86" t="s">
         <v>138</v>
-      </c>
-      <c r="J12" s="86" t="s">
-        <v>139</v>
       </c>
       <c r="L12" s="86"/>
     </row>
@@ -3071,7 +3092,7 @@
     <row r="15" spans="2:12" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:12" ht="13" x14ac:dyDescent="0.3">
       <c r="C16" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D16" s="66" t="s">
         <v>27</v>
@@ -3100,7 +3121,7 @@
     </row>
     <row r="17" spans="3:11" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="76" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D17" s="74" t="s">
         <v>6</v>
@@ -3115,13 +3136,13 @@
         <v>100</v>
       </c>
       <c r="H17" s="74" t="s">
+        <v>139</v>
+      </c>
+      <c r="I17" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="I17" s="75" t="s">
+      <c r="J17" s="74" t="s">
         <v>141</v>
-      </c>
-      <c r="J17" s="74" t="s">
-        <v>142</v>
       </c>
       <c r="K17" s="75" t="s">
         <v>95</v>
@@ -3129,45 +3150,45 @@
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C20" s="91" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D20" s="93" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C22" s="87" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C24" s="90" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C25" s="92" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C26" s="92" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C28" s="87" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C29" s="91" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C30" s="91" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D30" s="86">
         <v>0.8</v>

</xml_diff>